<commit_message>
Updated tests and books
</commit_message>
<xml_diff>
--- a/book/tests/test_all_criteria.xlsx
+++ b/book/tests/test_all_criteria.xlsx
@@ -10,8 +10,8 @@
     <sheet name="readme" sheetId="1" r:id="rId1"/>
     <sheet name="Criteria Failing, Air Speed 0.1" sheetId="2" r:id="rId2"/>
     <sheet name="Criterion 2, Air Speed 0.1" sheetId="3" r:id="rId3"/>
-    <sheet name="Criterion 3, Air Speed 0.1" sheetId="4" r:id="rId4"/>
-    <sheet name="Criterion 1, Air Speed 0.1" sheetId="5" r:id="rId5"/>
+    <sheet name="Criterion 1, Air Speed 0.1" sheetId="4" r:id="rId4"/>
+    <sheet name="Criterion 3, Air Speed 0.1" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -20,18 +20,18 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="58">
   <si>
+    <t>JobNo</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Author</t>
+  </si>
+  <si>
     <t>sheet_name</t>
   </si>
   <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>JobNo</t>
-  </si>
-  <si>
-    <t>Author</t>
-  </si>
-  <si>
     <t>0</t>
   </si>
   <si>
@@ -44,27 +44,27 @@
     <t>3</t>
   </si>
   <si>
+    <t>/c/e</t>
+  </si>
+  <si>
+    <t>20220228</t>
+  </si>
+  <si>
+    <t>jovyan</t>
+  </si>
+  <si>
     <t>Criteria Failing, Air Speed 0.1</t>
   </si>
   <si>
     <t>Criterion 2, Air Speed 0.1</t>
   </si>
   <si>
+    <t>Criterion 1, Air Speed 0.1</t>
+  </si>
+  <si>
     <t>Criterion 3, Air Speed 0.1</t>
   </si>
   <si>
-    <t>Criterion 1, Air Speed 0.1</t>
-  </si>
-  <si>
-    <t>20220224</t>
-  </si>
-  <si>
-    <t>/c/e</t>
-  </si>
-  <si>
-    <t>jovyan</t>
-  </si>
-  <si>
     <t>index</t>
   </si>
   <si>
@@ -182,16 +182,16 @@
     <t>Criterion 2 Relative Change (%)</t>
   </si>
   <si>
+    <t>Criterion 1 Absolute Change</t>
+  </si>
+  <si>
+    <t>Criterion 1 Relative Change (%)</t>
+  </si>
+  <si>
     <t>Criterion 3 Absolute Change</t>
   </si>
   <si>
     <t>Criterion 3 Relative Change (%)</t>
-  </si>
-  <si>
-    <t>Criterion 1 Absolute Change</t>
-  </si>
-  <si>
-    <t>Criterion 1 Relative Change (%)</t>
   </si>
 </sst>
 </file>
@@ -375,10 +375,10 @@
   <autoFilter ref="A1:E5"/>
   <tableColumns count="5">
     <tableColumn id="1" name="index"/>
-    <tableColumn id="2" name="sheet_name"/>
+    <tableColumn id="2" name="JobNo"/>
     <tableColumn id="3" name="Date"/>
-    <tableColumn id="4" name="JobNo"/>
-    <tableColumn id="5" name="Author"/>
+    <tableColumn id="4" name="Author"/>
+    <tableColumn id="5" name="sheet_name"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -421,8 +421,8 @@
     <tableColumn id="2" name="Room Name"/>
     <tableColumn id="3" name="IES Results"/>
     <tableColumn id="4" name="MF Results"/>
-    <tableColumn id="5" name="Criterion 3 Absolute Change"/>
-    <tableColumn id="6" name="Criterion 3 Relative Change (%)"/>
+    <tableColumn id="5" name="Criterion 1 Absolute Change"/>
+    <tableColumn id="6" name="Criterion 1 Relative Change (%)"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -436,8 +436,8 @@
     <tableColumn id="2" name="Room Name"/>
     <tableColumn id="3" name="IES Results"/>
     <tableColumn id="4" name="MF Results"/>
-    <tableColumn id="5" name="Criterion 1 Absolute Change"/>
-    <tableColumn id="6" name="Criterion 1 Relative Change (%)"/>
+    <tableColumn id="5" name="Criterion 3 Absolute Change"/>
+    <tableColumn id="6" name="Criterion 3 Relative Change (%)"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -768,13 +768,13 @@
         <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -782,16 +782,16 @@
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -799,16 +799,16 @@
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -816,13 +816,13 @@
         <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>14</v>
@@ -1990,10 +1990,10 @@
         <v>20</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="D2">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -2010,16 +2010,16 @@
         <v>21</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>7.8</v>
       </c>
       <c r="D3">
-        <v>2</v>
+        <v>7.9</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>0.1000000000000005</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>1.282051282051289</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -2030,16 +2030,16 @@
         <v>22</v>
       </c>
       <c r="C4">
-        <v>2</v>
+        <v>8.1</v>
       </c>
       <c r="D4">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>-0.09999999999999964</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>-1.234567901234563</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -2118,10 +2118,10 @@
         <v>27</v>
       </c>
       <c r="C9">
-        <v>3</v>
+        <v>10.6</v>
       </c>
       <c r="D9">
-        <v>3</v>
+        <v>10.6</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -2138,10 +2138,10 @@
         <v>28</v>
       </c>
       <c r="C10">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="D10">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -2158,10 +2158,10 @@
         <v>29</v>
       </c>
       <c r="C11">
-        <v>3</v>
+        <v>11.6</v>
       </c>
       <c r="D11">
-        <v>3</v>
+        <v>11.6</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -2178,16 +2178,16 @@
         <v>30</v>
       </c>
       <c r="C12">
-        <v>3</v>
+        <v>26.3</v>
       </c>
       <c r="D12">
-        <v>3</v>
+        <v>26.4</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>0.09999999999999787</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <v>0.3802281368821211</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -2215,10 +2215,10 @@
         <v>32</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="D14">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="E14">
         <v>0</v>
@@ -2235,10 +2235,10 @@
         <v>33</v>
       </c>
       <c r="C15">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="D15">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -2272,10 +2272,10 @@
         <v>35</v>
       </c>
       <c r="C17">
-        <v>3</v>
+        <v>12.9</v>
       </c>
       <c r="D17">
-        <v>3</v>
+        <v>12.9</v>
       </c>
       <c r="E17">
         <v>0</v>
@@ -2292,10 +2292,10 @@
         <v>36</v>
       </c>
       <c r="C18">
-        <v>3</v>
+        <v>28.3</v>
       </c>
       <c r="D18">
-        <v>3</v>
+        <v>28.3</v>
       </c>
       <c r="E18">
         <v>0</v>
@@ -2312,16 +2312,16 @@
         <v>37</v>
       </c>
       <c r="C19">
-        <v>3</v>
+        <v>13.4</v>
       </c>
       <c r="D19">
-        <v>3</v>
+        <v>13.5</v>
       </c>
       <c r="E19">
-        <v>0</v>
+        <v>0.09999999999999964</v>
       </c>
       <c r="F19">
-        <v>0</v>
+        <v>0.7462686567164152</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -2332,16 +2332,16 @@
         <v>38</v>
       </c>
       <c r="C20">
-        <v>3</v>
+        <v>28.6</v>
       </c>
       <c r="D20">
-        <v>3</v>
+        <v>28.5</v>
       </c>
       <c r="E20">
-        <v>0</v>
+        <v>-0.1000000000000014</v>
       </c>
       <c r="F20">
-        <v>0</v>
+        <v>-0.3496503496503546</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -2352,15 +2352,12 @@
         <v>39</v>
       </c>
       <c r="C21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E21">
-        <v>0</v>
-      </c>
-      <c r="F21">
         <v>0</v>
       </c>
     </row>
@@ -2372,10 +2369,10 @@
         <v>40</v>
       </c>
       <c r="C22">
-        <v>1</v>
+        <v>1.6</v>
       </c>
       <c r="D22">
-        <v>1</v>
+        <v>1.6</v>
       </c>
       <c r="E22">
         <v>0</v>
@@ -2392,10 +2389,10 @@
         <v>41</v>
       </c>
       <c r="C23">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="D23">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="E23">
         <v>0</v>
@@ -2412,15 +2409,12 @@
         <v>42</v>
       </c>
       <c r="C24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E24">
-        <v>0</v>
-      </c>
-      <c r="F24">
         <v>0</v>
       </c>
     </row>
@@ -2432,10 +2426,10 @@
         <v>43</v>
       </c>
       <c r="C25">
-        <v>2</v>
+        <v>5.6</v>
       </c>
       <c r="D25">
-        <v>2</v>
+        <v>5.6</v>
       </c>
       <c r="E25">
         <v>0</v>
@@ -2452,16 +2446,16 @@
         <v>44</v>
       </c>
       <c r="C26">
-        <v>2</v>
+        <v>17.7</v>
       </c>
       <c r="D26">
-        <v>2</v>
+        <v>17.8</v>
       </c>
       <c r="E26">
-        <v>0</v>
+        <v>0.1000000000000014</v>
       </c>
       <c r="F26">
-        <v>0</v>
+        <v>0.5649717514124375</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -2472,10 +2466,10 @@
         <v>45</v>
       </c>
       <c r="C27">
-        <v>2</v>
+        <v>5.2</v>
       </c>
       <c r="D27">
-        <v>2</v>
+        <v>5.2</v>
       </c>
       <c r="E27">
         <v>0</v>
@@ -2492,10 +2486,10 @@
         <v>46</v>
       </c>
       <c r="C28">
-        <v>2</v>
+        <v>17.7</v>
       </c>
       <c r="D28">
-        <v>2</v>
+        <v>17.7</v>
       </c>
       <c r="E28">
         <v>0</v>
@@ -2621,10 +2615,10 @@
         <v>20</v>
       </c>
       <c r="C2">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="D2">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -2641,16 +2635,16 @@
         <v>21</v>
       </c>
       <c r="C3">
-        <v>7.8</v>
+        <v>2</v>
       </c>
       <c r="D3">
-        <v>7.9</v>
+        <v>2</v>
       </c>
       <c r="E3">
-        <v>0.1000000000000005</v>
+        <v>0</v>
       </c>
       <c r="F3">
-        <v>1.282051282051289</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -2661,16 +2655,16 @@
         <v>22</v>
       </c>
       <c r="C4">
-        <v>8.1</v>
+        <v>2</v>
       </c>
       <c r="D4">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E4">
-        <v>0.09999999999999964</v>
+        <v>0</v>
       </c>
       <c r="F4">
-        <v>1.234567901234563</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -2749,10 +2743,10 @@
         <v>27</v>
       </c>
       <c r="C9">
-        <v>10.6</v>
+        <v>3</v>
       </c>
       <c r="D9">
-        <v>10.6</v>
+        <v>3</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -2769,10 +2763,10 @@
         <v>28</v>
       </c>
       <c r="C10">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="D10">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -2789,10 +2783,10 @@
         <v>29</v>
       </c>
       <c r="C11">
-        <v>11.6</v>
+        <v>3</v>
       </c>
       <c r="D11">
-        <v>11.6</v>
+        <v>3</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -2809,16 +2803,16 @@
         <v>30</v>
       </c>
       <c r="C12">
-        <v>26.3</v>
+        <v>3</v>
       </c>
       <c r="D12">
-        <v>26.4</v>
+        <v>3</v>
       </c>
       <c r="E12">
-        <v>0.09999999999999787</v>
+        <v>0</v>
       </c>
       <c r="F12">
-        <v>0.3802281368821211</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -2846,10 +2840,10 @@
         <v>32</v>
       </c>
       <c r="C14">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="D14">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="E14">
         <v>0</v>
@@ -2866,10 +2860,10 @@
         <v>33</v>
       </c>
       <c r="C15">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D15">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -2903,10 +2897,10 @@
         <v>35</v>
       </c>
       <c r="C17">
-        <v>12.9</v>
+        <v>3</v>
       </c>
       <c r="D17">
-        <v>12.9</v>
+        <v>3</v>
       </c>
       <c r="E17">
         <v>0</v>
@@ -2923,10 +2917,10 @@
         <v>36</v>
       </c>
       <c r="C18">
-        <v>28.3</v>
+        <v>3</v>
       </c>
       <c r="D18">
-        <v>28.3</v>
+        <v>3</v>
       </c>
       <c r="E18">
         <v>0</v>
@@ -2943,16 +2937,16 @@
         <v>37</v>
       </c>
       <c r="C19">
-        <v>13.4</v>
+        <v>3</v>
       </c>
       <c r="D19">
-        <v>13.5</v>
+        <v>3</v>
       </c>
       <c r="E19">
-        <v>0.09999999999999964</v>
+        <v>0</v>
       </c>
       <c r="F19">
-        <v>0.7462686567164152</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -2963,16 +2957,16 @@
         <v>38</v>
       </c>
       <c r="C20">
-        <v>28.6</v>
+        <v>3</v>
       </c>
       <c r="D20">
-        <v>28.5</v>
+        <v>3</v>
       </c>
       <c r="E20">
-        <v>0.1000000000000014</v>
+        <v>0</v>
       </c>
       <c r="F20">
-        <v>0.3496503496503546</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -2983,12 +2977,15 @@
         <v>39</v>
       </c>
       <c r="C21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
         <v>0</v>
       </c>
     </row>
@@ -3000,10 +2997,10 @@
         <v>40</v>
       </c>
       <c r="C22">
-        <v>1.6</v>
+        <v>1</v>
       </c>
       <c r="D22">
-        <v>1.6</v>
+        <v>1</v>
       </c>
       <c r="E22">
         <v>0</v>
@@ -3020,10 +3017,10 @@
         <v>41</v>
       </c>
       <c r="C23">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="D23">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="E23">
         <v>0</v>
@@ -3040,12 +3037,15 @@
         <v>42</v>
       </c>
       <c r="C24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
         <v>0</v>
       </c>
     </row>
@@ -3057,10 +3057,10 @@
         <v>43</v>
       </c>
       <c r="C25">
-        <v>5.6</v>
+        <v>2</v>
       </c>
       <c r="D25">
-        <v>5.6</v>
+        <v>2</v>
       </c>
       <c r="E25">
         <v>0</v>
@@ -3077,16 +3077,16 @@
         <v>44</v>
       </c>
       <c r="C26">
-        <v>17.7</v>
+        <v>2</v>
       </c>
       <c r="D26">
-        <v>17.8</v>
+        <v>2</v>
       </c>
       <c r="E26">
-        <v>0.1000000000000014</v>
+        <v>0</v>
       </c>
       <c r="F26">
-        <v>0.5649717514124375</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -3097,10 +3097,10 @@
         <v>45</v>
       </c>
       <c r="C27">
-        <v>5.2</v>
+        <v>2</v>
       </c>
       <c r="D27">
-        <v>5.2</v>
+        <v>2</v>
       </c>
       <c r="E27">
         <v>0</v>
@@ -3117,10 +3117,10 @@
         <v>46</v>
       </c>
       <c r="C28">
-        <v>17.7</v>
+        <v>2</v>
       </c>
       <c r="D28">
-        <v>17.7</v>
+        <v>2</v>
       </c>
       <c r="E28">
         <v>0</v>

</xml_diff>